<commit_message>
fixed order 6 again
changes not saving on all computers
</commit_message>
<xml_diff>
--- a/Experiment/Orders_PILOT/PAR01_RUN06.xlsx
+++ b/Experiment/Orders_PILOT/PAR01_RUN06.xlsx
@@ -580,8 +580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A177" workbookViewId="0">
-      <selection activeCell="F177" sqref="F1:F1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="H138" sqref="H138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2869,10 +2869,10 @@
         <v>1</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="F108" t="b">
         <v>0</v>
@@ -3289,10 +3289,10 @@
         <v>5</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="F129" t="b">
         <v>0</v>

</xml_diff>